<commit_message>
Add excel eval dataset
</commit_message>
<xml_diff>
--- a/rag/eval_dataset_handcrafted.xlsx
+++ b/rag/eval_dataset_handcrafted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LNshuti\OneDrive - Sony\Desktop\learn\metals-trade\rag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{135E231F-AF1F-4D22-B88F-FEB9842BBB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE742408-144E-4B0B-B100-3F4D1E0DF043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31785" yWindow="2250" windowWidth="21600" windowHeight="11325" xr2:uid="{3774AE54-E282-48A7-9A1F-24446D336CB8}"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="19200" windowHeight="10725" xr2:uid="{3774AE54-E282-48A7-9A1F-24446D336CB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>query</t>
   </si>
@@ -69,6 +69,30 @@
   </si>
   <si>
     <t>The US Geological Survey(USGS) and the US Department of Energy</t>
+  </si>
+  <si>
+    <t>Which minerals are on both the US Geological Survey and the Department of Energy's lists of critical minerals?</t>
+  </si>
+  <si>
+    <t>Cobalt, Graphite, Lithium, Manganese and Nickel</t>
+  </si>
+  <si>
+    <t>Which country is the leading producer of cobalt?</t>
+  </si>
+  <si>
+    <t>The Democratic Republic of Congo</t>
+  </si>
+  <si>
+    <t>Which country is the leading producer of Lithium?</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Which country is the leading producer of rare earth minerals</t>
+  </si>
+  <si>
+    <t>China</t>
   </si>
 </sst>
 </file>
@@ -429,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825A05CC-5C07-477E-B452-00B307DD5FE8}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,6 +510,38 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>